<commit_message>
Corrected DSP Feedermap in DataSet
</commit_message>
<xml_diff>
--- a/AutoFirmwareUpgrade/CashelFirmwareAutomatedTest/TestDataFiles/CablingDataSet/1U4U3I.xlsx
+++ b/AutoFirmwareUpgrade/CashelFirmwareAutomatedTest/TestDataFiles/CablingDataSet/1U4U3I.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9114372F-0D91-4AEA-B9B8-052606D5890B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04A0285-BDA1-4E14-8204-CAB212AC82FF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DeviceInfo" sheetId="3" r:id="rId1"/>
@@ -1577,11 +1577,14 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -1612,7 +1615,7 @@
         <v>127</v>
       </c>
       <c r="B4" s="2">
-        <v>2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1620,7 +1623,7 @@
         <v>128</v>
       </c>
       <c r="B5" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1628,7 +1631,7 @@
         <v>129</v>
       </c>
       <c r="B6" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1996,7 +1999,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>